<commit_message>
fixed a small issue
</commit_message>
<xml_diff>
--- a/perceptron output.xlsx
+++ b/perceptron output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL352"/>
+  <dimension ref="A1:AK352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,11 +611,6 @@
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
           <t>predicted</t>
         </is>
       </c>
@@ -731,10 +726,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -851,10 +843,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL3" t="inlineStr">
+      <c r="AK3" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -971,10 +960,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL4" t="inlineStr">
+      <c r="AK4" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -1091,10 +1077,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL5" t="inlineStr">
+      <c r="AK5" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -1211,10 +1194,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL6" t="inlineStr">
+      <c r="AK6" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -1331,10 +1311,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL7" t="inlineStr">
+      <c r="AK7" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -1451,10 +1428,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL8" t="inlineStr">
+      <c r="AK8" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -1571,10 +1545,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL9" t="inlineStr">
+      <c r="AK9" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -1691,10 +1662,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL10" t="inlineStr">
+      <c r="AK10" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -1811,10 +1779,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL11" t="inlineStr">
+      <c r="AK11" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -1931,10 +1896,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL12" t="inlineStr">
+      <c r="AK12" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -2051,10 +2013,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL13" t="inlineStr">
+      <c r="AK13" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -2171,10 +2130,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL14" t="inlineStr">
+      <c r="AK14" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -2291,10 +2247,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL15" t="inlineStr">
+      <c r="AK15" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -2411,10 +2364,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL16" t="inlineStr">
+      <c r="AK16" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -2531,10 +2481,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL17" t="inlineStr">
+      <c r="AK17" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -2651,10 +2598,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL18" t="inlineStr">
+      <c r="AK18" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -2771,10 +2715,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL19" t="inlineStr">
+      <c r="AK19" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -2891,10 +2832,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL20" t="inlineStr">
+      <c r="AK20" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -3011,10 +2949,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL21" t="inlineStr">
+      <c r="AK21" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -3131,10 +3066,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL22" t="inlineStr">
+      <c r="AK22" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -3251,10 +3183,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL23" t="inlineStr">
+      <c r="AK23" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -3371,10 +3300,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL24" t="inlineStr">
+      <c r="AK24" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -3491,10 +3417,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL25" t="inlineStr">
+      <c r="AK25" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -3611,10 +3534,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK26" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL26" t="inlineStr">
+      <c r="AK26" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -3731,10 +3651,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL27" t="inlineStr">
+      <c r="AK27" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -3851,10 +3768,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL28" t="inlineStr">
+      <c r="AK28" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -3971,10 +3885,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK29" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL29" t="inlineStr">
+      <c r="AK29" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -4091,10 +4002,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK30" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL30" t="inlineStr">
+      <c r="AK30" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -4211,10 +4119,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL31" t="inlineStr">
+      <c r="AK31" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -4331,10 +4236,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK32" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL32" t="inlineStr">
+      <c r="AK32" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -4451,10 +4353,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK33" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL33" t="inlineStr">
+      <c r="AK33" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -4571,10 +4470,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL34" t="inlineStr">
+      <c r="AK34" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -4691,10 +4587,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL35" t="inlineStr">
+      <c r="AK35" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -4811,10 +4704,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL36" t="inlineStr">
+      <c r="AK36" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -4931,10 +4821,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL37" t="inlineStr">
+      <c r="AK37" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -5051,10 +4938,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK38" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL38" t="inlineStr">
+      <c r="AK38" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -5171,10 +5055,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK39" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL39" t="inlineStr">
+      <c r="AK39" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -5291,10 +5172,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK40" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL40" t="inlineStr">
+      <c r="AK40" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -5411,10 +5289,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK41" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL41" t="inlineStr">
+      <c r="AK41" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -5531,10 +5406,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK42" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL42" t="inlineStr">
+      <c r="AK42" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -5651,10 +5523,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK43" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL43" t="inlineStr">
+      <c r="AK43" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -5771,10 +5640,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK44" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL44" t="inlineStr">
+      <c r="AK44" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -5891,10 +5757,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL45" t="inlineStr">
+      <c r="AK45" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -6011,10 +5874,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL46" t="inlineStr">
+      <c r="AK46" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -6131,10 +5991,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL47" t="inlineStr">
+      <c r="AK47" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -6251,10 +6108,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL48" t="inlineStr">
+      <c r="AK48" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -6371,10 +6225,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK49" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL49" t="inlineStr">
+      <c r="AK49" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -6491,10 +6342,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL50" t="inlineStr">
+      <c r="AK50" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -6611,10 +6459,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK51" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL51" t="inlineStr">
+      <c r="AK51" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -6731,10 +6576,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK52" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL52" t="inlineStr">
+      <c r="AK52" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -6851,10 +6693,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK53" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL53" t="inlineStr">
+      <c r="AK53" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -6971,10 +6810,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK54" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL54" t="inlineStr">
+      <c r="AK54" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -7091,10 +6927,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK55" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL55" t="inlineStr">
+      <c r="AK55" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -7211,10 +7044,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK56" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL56" t="inlineStr">
+      <c r="AK56" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -7331,10 +7161,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK57" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL57" t="inlineStr">
+      <c r="AK57" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -7451,10 +7278,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK58" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL58" t="inlineStr">
+      <c r="AK58" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -7571,10 +7395,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK59" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL59" t="inlineStr">
+      <c r="AK59" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -7691,10 +7512,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK60" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL60" t="inlineStr">
+      <c r="AK60" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -7811,10 +7629,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK61" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL61" t="inlineStr">
+      <c r="AK61" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -7931,10 +7746,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL62" t="inlineStr">
+      <c r="AK62" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -8051,10 +7863,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL63" t="inlineStr">
+      <c r="AK63" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -8171,10 +7980,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK64" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL64" t="inlineStr">
+      <c r="AK64" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -8291,10 +8097,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK65" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL65" t="inlineStr">
+      <c r="AK65" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -8411,10 +8214,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK66" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL66" t="inlineStr">
+      <c r="AK66" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -8531,10 +8331,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK67" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL67" t="inlineStr">
+      <c r="AK67" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -8651,10 +8448,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK68" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL68" t="inlineStr">
+      <c r="AK68" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -8771,10 +8565,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK69" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL69" t="inlineStr">
+      <c r="AK69" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -8891,10 +8682,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK70" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL70" t="inlineStr">
+      <c r="AK70" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -9011,10 +8799,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK71" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL71" t="inlineStr">
+      <c r="AK71" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -9131,10 +8916,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK72" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL72" t="inlineStr">
+      <c r="AK72" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -9251,10 +9033,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK73" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL73" t="inlineStr">
+      <c r="AK73" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -9371,10 +9150,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK74" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL74" t="inlineStr">
+      <c r="AK74" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -9491,10 +9267,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK75" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL75" t="inlineStr">
+      <c r="AK75" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -9611,10 +9384,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK76" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL76" t="inlineStr">
+      <c r="AK76" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -9731,10 +9501,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK77" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL77" t="inlineStr">
+      <c r="AK77" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -9851,10 +9618,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK78" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL78" t="inlineStr">
+      <c r="AK78" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -9971,10 +9735,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL79" t="inlineStr">
+      <c r="AK79" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -10091,10 +9852,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL80" t="inlineStr">
+      <c r="AK80" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -10211,10 +9969,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK81" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL81" t="inlineStr">
+      <c r="AK81" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -10331,10 +10086,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK82" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL82" t="inlineStr">
+      <c r="AK82" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -10451,10 +10203,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK83" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL83" t="inlineStr">
+      <c r="AK83" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -10571,10 +10320,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK84" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL84" t="inlineStr">
+      <c r="AK84" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -10691,10 +10437,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK85" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL85" t="inlineStr">
+      <c r="AK85" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -10811,10 +10554,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK86" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL86" t="inlineStr">
+      <c r="AK86" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -10931,10 +10671,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL87" t="inlineStr">
+      <c r="AK87" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -11051,10 +10788,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK88" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL88" t="inlineStr">
+      <c r="AK88" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -11171,10 +10905,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK89" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL89" t="inlineStr">
+      <c r="AK89" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -11291,10 +11022,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK90" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL90" t="inlineStr">
+      <c r="AK90" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -11411,10 +11139,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK91" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL91" t="inlineStr">
+      <c r="AK91" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -11531,10 +11256,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK92" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL92" t="inlineStr">
+      <c r="AK92" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -11651,10 +11373,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK93" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL93" t="inlineStr">
+      <c r="AK93" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -11771,10 +11490,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK94" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL94" t="inlineStr">
+      <c r="AK94" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -11891,10 +11607,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK95" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL95" t="inlineStr">
+      <c r="AK95" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -12011,10 +11724,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL96" t="inlineStr">
+      <c r="AK96" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12131,10 +11841,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL97" t="inlineStr">
+      <c r="AK97" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12251,10 +11958,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK98" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL98" t="inlineStr">
+      <c r="AK98" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12371,10 +12075,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK99" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL99" t="inlineStr">
+      <c r="AK99" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12491,10 +12192,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK100" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL100" t="inlineStr">
+      <c r="AK100" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12611,10 +12309,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK101" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL101" t="inlineStr">
+      <c r="AK101" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12731,10 +12426,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK102" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL102" t="inlineStr">
+      <c r="AK102" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12851,10 +12543,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK103" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL103" t="inlineStr">
+      <c r="AK103" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -12971,10 +12660,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK104" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL104" t="inlineStr">
+      <c r="AK104" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -13091,10 +12777,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK105" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL105" t="inlineStr">
+      <c r="AK105" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -13211,10 +12894,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK106" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL106" t="inlineStr">
+      <c r="AK106" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -13331,10 +13011,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK107" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL107" t="inlineStr">
+      <c r="AK107" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -13451,10 +13128,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK108" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL108" t="inlineStr">
+      <c r="AK108" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -13571,10 +13245,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK109" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL109" t="inlineStr">
+      <c r="AK109" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -13691,10 +13362,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK110" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL110" t="inlineStr">
+      <c r="AK110" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -13811,10 +13479,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK111" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL111" t="inlineStr">
+      <c r="AK111" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -13931,10 +13596,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK112" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL112" t="inlineStr">
+      <c r="AK112" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -14051,10 +13713,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK113" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL113" t="inlineStr">
+      <c r="AK113" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -14171,10 +13830,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK114" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL114" t="inlineStr">
+      <c r="AK114" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -14291,10 +13947,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK115" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL115" t="inlineStr">
+      <c r="AK115" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -14411,10 +14064,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK116" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL116" t="inlineStr">
+      <c r="AK116" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -14531,10 +14181,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK117" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL117" t="inlineStr">
+      <c r="AK117" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -14651,10 +14298,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL118" t="inlineStr">
+      <c r="AK118" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -14771,10 +14415,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK119" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL119" t="inlineStr">
+      <c r="AK119" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -14891,10 +14532,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK120" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL120" t="inlineStr">
+      <c r="AK120" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -15011,10 +14649,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK121" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL121" t="inlineStr">
+      <c r="AK121" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -15131,10 +14766,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK122" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL122" t="inlineStr">
+      <c r="AK122" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -15251,10 +14883,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK123" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL123" t="inlineStr">
+      <c r="AK123" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -15371,10 +15000,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK124" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL124" t="inlineStr">
+      <c r="AK124" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -15491,10 +15117,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK125" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL125" t="inlineStr">
+      <c r="AK125" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -15611,10 +15234,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK126" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL126" t="inlineStr">
+      <c r="AK126" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -15731,10 +15351,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK127" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL127" t="inlineStr">
+      <c r="AK127" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -15851,10 +15468,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK128" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL128" t="inlineStr">
+      <c r="AK128" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -15971,10 +15585,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK129" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL129" t="inlineStr">
+      <c r="AK129" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -16091,10 +15702,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK130" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL130" t="inlineStr">
+      <c r="AK130" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -16211,10 +15819,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK131" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL131" t="inlineStr">
+      <c r="AK131" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -16331,10 +15936,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK132" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL132" t="inlineStr">
+      <c r="AK132" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -16451,10 +16053,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK133" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL133" t="inlineStr">
+      <c r="AK133" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -16571,10 +16170,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK134" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL134" t="inlineStr">
+      <c r="AK134" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -16691,10 +16287,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK135" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL135" t="inlineStr">
+      <c r="AK135" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -16811,10 +16404,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK136" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL136" t="inlineStr">
+      <c r="AK136" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -16931,10 +16521,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK137" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL137" t="inlineStr">
+      <c r="AK137" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -17051,10 +16638,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK138" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL138" t="inlineStr">
+      <c r="AK138" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -17171,10 +16755,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK139" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL139" t="inlineStr">
+      <c r="AK139" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -17291,10 +16872,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL140" t="inlineStr">
+      <c r="AK140" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -17411,10 +16989,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL141" t="inlineStr">
+      <c r="AK141" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -17531,10 +17106,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK142" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL142" t="inlineStr">
+      <c r="AK142" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -17651,10 +17223,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK143" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL143" t="inlineStr">
+      <c r="AK143" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -17771,10 +17340,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK144" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL144" t="inlineStr">
+      <c r="AK144" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -17891,10 +17457,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK145" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL145" t="inlineStr">
+      <c r="AK145" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -18011,10 +17574,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK146" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL146" t="inlineStr">
+      <c r="AK146" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -18131,10 +17691,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK147" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL147" t="inlineStr">
+      <c r="AK147" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -18251,10 +17808,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK148" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL148" t="inlineStr">
+      <c r="AK148" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -18371,10 +17925,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK149" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL149" t="inlineStr">
+      <c r="AK149" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -18491,10 +18042,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK150" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL150" t="inlineStr">
+      <c r="AK150" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -18611,10 +18159,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK151" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL151" t="inlineStr">
+      <c r="AK151" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -18731,10 +18276,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK152" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL152" t="inlineStr">
+      <c r="AK152" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -18851,10 +18393,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK153" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL153" t="inlineStr">
+      <c r="AK153" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -18971,10 +18510,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK154" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL154" t="inlineStr">
+      <c r="AK154" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -19091,10 +18627,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK155" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL155" t="inlineStr">
+      <c r="AK155" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -19211,10 +18744,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK156" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL156" t="inlineStr">
+      <c r="AK156" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -19331,10 +18861,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK157" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL157" t="inlineStr">
+      <c r="AK157" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -19451,10 +18978,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK158" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL158" t="inlineStr">
+      <c r="AK158" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -19571,10 +19095,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK159" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL159" t="inlineStr">
+      <c r="AK159" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -19691,10 +19212,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK160" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL160" t="inlineStr">
+      <c r="AK160" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -19811,10 +19329,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK161" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL161" t="inlineStr">
+      <c r="AK161" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -19931,10 +19446,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK162" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL162" t="inlineStr">
+      <c r="AK162" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -20051,10 +19563,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK163" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL163" t="inlineStr">
+      <c r="AK163" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -20171,10 +19680,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK164" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL164" t="inlineStr">
+      <c r="AK164" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -20291,10 +19797,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK165" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL165" t="inlineStr">
+      <c r="AK165" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -20411,10 +19914,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK166" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL166" t="inlineStr">
+      <c r="AK166" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -20531,10 +20031,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK167" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL167" t="inlineStr">
+      <c r="AK167" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -20651,10 +20148,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK168" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL168" t="inlineStr">
+      <c r="AK168" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -20771,10 +20265,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK169" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL169" t="inlineStr">
+      <c r="AK169" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -20891,10 +20382,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK170" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL170" t="inlineStr">
+      <c r="AK170" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -21011,10 +20499,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK171" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL171" t="inlineStr">
+      <c r="AK171" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -21131,10 +20616,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK172" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL172" t="inlineStr">
+      <c r="AK172" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -21251,10 +20733,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK173" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL173" t="inlineStr">
+      <c r="AK173" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -21371,10 +20850,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK174" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL174" t="inlineStr">
+      <c r="AK174" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -21491,10 +20967,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK175" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL175" t="inlineStr">
+      <c r="AK175" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -21611,10 +21084,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK176" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL176" t="inlineStr">
+      <c r="AK176" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -21731,10 +21201,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK177" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL177" t="inlineStr">
+      <c r="AK177" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -21851,10 +21318,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK178" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL178" t="inlineStr">
+      <c r="AK178" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -21971,10 +21435,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK179" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL179" t="inlineStr">
+      <c r="AK179" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -22091,10 +21552,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK180" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL180" t="inlineStr">
+      <c r="AK180" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -22211,10 +21669,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK181" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL181" t="inlineStr">
+      <c r="AK181" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -22331,10 +21786,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK182" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL182" t="inlineStr">
+      <c r="AK182" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -22451,10 +21903,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK183" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL183" t="inlineStr">
+      <c r="AK183" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -22571,10 +22020,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK184" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL184" t="inlineStr">
+      <c r="AK184" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -22691,10 +22137,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK185" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL185" t="inlineStr">
+      <c r="AK185" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -22811,10 +22254,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK186" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL186" t="inlineStr">
+      <c r="AK186" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -22931,10 +22371,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK187" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL187" t="inlineStr">
+      <c r="AK187" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -23051,10 +22488,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK188" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL188" t="inlineStr">
+      <c r="AK188" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -23171,10 +22605,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK189" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL189" t="inlineStr">
+      <c r="AK189" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -23291,10 +22722,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK190" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL190" t="inlineStr">
+      <c r="AK190" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -23411,10 +22839,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK191" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL191" t="inlineStr">
+      <c r="AK191" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -23531,10 +22956,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK192" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL192" t="inlineStr">
+      <c r="AK192" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -23651,10 +23073,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK193" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL193" t="inlineStr">
+      <c r="AK193" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -23771,10 +23190,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK194" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL194" t="inlineStr">
+      <c r="AK194" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -23891,10 +23307,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK195" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL195" t="inlineStr">
+      <c r="AK195" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -24011,10 +23424,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK196" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL196" t="inlineStr">
+      <c r="AK196" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -24131,10 +23541,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK197" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL197" t="inlineStr">
+      <c r="AK197" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -24251,10 +23658,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK198" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL198" t="inlineStr">
+      <c r="AK198" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -24371,10 +23775,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK199" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL199" t="inlineStr">
+      <c r="AK199" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -24491,10 +23892,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK200" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL200" t="inlineStr">
+      <c r="AK200" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -24611,10 +24009,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK201" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL201" t="inlineStr">
+      <c r="AK201" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -24731,10 +24126,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK202" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL202" t="inlineStr">
+      <c r="AK202" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -24851,10 +24243,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK203" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL203" t="inlineStr">
+      <c r="AK203" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -24971,10 +24360,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK204" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL204" t="inlineStr">
+      <c r="AK204" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -25091,10 +24477,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK205" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL205" t="inlineStr">
+      <c r="AK205" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -25211,10 +24594,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK206" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL206" t="inlineStr">
+      <c r="AK206" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -25331,10 +24711,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK207" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL207" t="inlineStr">
+      <c r="AK207" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -25451,10 +24828,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK208" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL208" t="inlineStr">
+      <c r="AK208" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -25571,10 +24945,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK209" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL209" t="inlineStr">
+      <c r="AK209" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -25691,10 +25062,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK210" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL210" t="inlineStr">
+      <c r="AK210" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -25811,10 +25179,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK211" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL211" t="inlineStr">
+      <c r="AK211" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -25931,10 +25296,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK212" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL212" t="inlineStr">
+      <c r="AK212" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -26051,10 +25413,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK213" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL213" t="inlineStr">
+      <c r="AK213" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -26171,10 +25530,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK214" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL214" t="inlineStr">
+      <c r="AK214" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -26291,10 +25647,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK215" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL215" t="inlineStr">
+      <c r="AK215" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -26411,10 +25764,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK216" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL216" t="inlineStr">
+      <c r="AK216" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -26531,10 +25881,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK217" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL217" t="inlineStr">
+      <c r="AK217" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -26651,10 +25998,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK218" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL218" t="inlineStr">
+      <c r="AK218" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -26771,10 +26115,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK219" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL219" t="inlineStr">
+      <c r="AK219" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -26891,10 +26232,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK220" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL220" t="inlineStr">
+      <c r="AK220" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -27011,10 +26349,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK221" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL221" t="inlineStr">
+      <c r="AK221" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -27131,10 +26466,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK222" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL222" t="inlineStr">
+      <c r="AK222" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -27251,10 +26583,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK223" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL223" t="inlineStr">
+      <c r="AK223" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -27371,10 +26700,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK224" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL224" t="inlineStr">
+      <c r="AK224" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -27491,10 +26817,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK225" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL225" t="inlineStr">
+      <c r="AK225" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -27611,10 +26934,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK226" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL226" t="inlineStr">
+      <c r="AK226" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -27731,10 +27051,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK227" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL227" t="inlineStr">
+      <c r="AK227" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -27851,10 +27168,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK228" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL228" t="inlineStr">
+      <c r="AK228" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -27971,10 +27285,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK229" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL229" t="inlineStr">
+      <c r="AK229" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -28091,10 +27402,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK230" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL230" t="inlineStr">
+      <c r="AK230" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -28211,10 +27519,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK231" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL231" t="inlineStr">
+      <c r="AK231" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -28331,10 +27636,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK232" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL232" t="inlineStr">
+      <c r="AK232" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -28451,10 +27753,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK233" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL233" t="inlineStr">
+      <c r="AK233" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -28571,10 +27870,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK234" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL234" t="inlineStr">
+      <c r="AK234" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -28691,10 +27987,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK235" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL235" t="inlineStr">
+      <c r="AK235" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -28811,10 +28104,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK236" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL236" t="inlineStr">
+      <c r="AK236" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -28931,10 +28221,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK237" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL237" t="inlineStr">
+      <c r="AK237" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -29051,10 +28338,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK238" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL238" t="inlineStr">
+      <c r="AK238" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -29171,10 +28455,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK239" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL239" t="inlineStr">
+      <c r="AK239" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -29291,10 +28572,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK240" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL240" t="inlineStr">
+      <c r="AK240" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -29411,10 +28689,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK241" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL241" t="inlineStr">
+      <c r="AK241" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -29531,10 +28806,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK242" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL242" t="inlineStr">
+      <c r="AK242" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -29651,10 +28923,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK243" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL243" t="inlineStr">
+      <c r="AK243" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -29771,10 +29040,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK244" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL244" t="inlineStr">
+      <c r="AK244" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -29891,10 +29157,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK245" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL245" t="inlineStr">
+      <c r="AK245" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -30011,10 +29274,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK246" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL246" t="inlineStr">
+      <c r="AK246" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -30131,10 +29391,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK247" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL247" t="inlineStr">
+      <c r="AK247" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -30251,10 +29508,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK248" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL248" t="inlineStr">
+      <c r="AK248" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -30371,10 +29625,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK249" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL249" t="inlineStr">
+      <c r="AK249" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -30491,10 +29742,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK250" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL250" t="inlineStr">
+      <c r="AK250" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -30611,10 +29859,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK251" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL251" t="inlineStr">
+      <c r="AK251" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -30731,10 +29976,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK252" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL252" t="inlineStr">
+      <c r="AK252" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -30851,10 +30093,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK253" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL253" t="inlineStr">
+      <c r="AK253" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -30971,10 +30210,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="AK254" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL254" t="inlineStr">
+      <c r="AK254" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -31091,10 +30327,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK255" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL255" t="inlineStr">
+      <c r="AK255" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -31211,10 +30444,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK256" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL256" t="inlineStr">
+      <c r="AK256" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -31331,10 +30561,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK257" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL257" t="inlineStr">
+      <c r="AK257" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -31451,10 +30678,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK258" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL258" t="inlineStr">
+      <c r="AK258" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -31571,10 +30795,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK259" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL259" t="inlineStr">
+      <c r="AK259" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -31691,10 +30912,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK260" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL260" t="inlineStr">
+      <c r="AK260" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -31811,10 +31029,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK261" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL261" t="inlineStr">
+      <c r="AK261" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -31931,10 +31146,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK262" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL262" t="inlineStr">
+      <c r="AK262" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32051,10 +31263,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK263" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL263" t="inlineStr">
+      <c r="AK263" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32171,10 +31380,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK264" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL264" t="inlineStr">
+      <c r="AK264" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32291,10 +31497,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK265" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL265" t="inlineStr">
+      <c r="AK265" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32411,10 +31614,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK266" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL266" t="inlineStr">
+      <c r="AK266" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32531,10 +31731,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK267" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL267" t="inlineStr">
+      <c r="AK267" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32651,10 +31848,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK268" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL268" t="inlineStr">
+      <c r="AK268" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32771,10 +31965,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK269" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL269" t="inlineStr">
+      <c r="AK269" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -32891,10 +32082,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK270" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL270" t="inlineStr">
+      <c r="AK270" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33011,10 +32199,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK271" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL271" t="inlineStr">
+      <c r="AK271" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33131,10 +32316,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK272" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL272" t="inlineStr">
+      <c r="AK272" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33251,10 +32433,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK273" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL273" t="inlineStr">
+      <c r="AK273" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33371,10 +32550,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK274" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL274" t="inlineStr">
+      <c r="AK274" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33491,10 +32667,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK275" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL275" t="inlineStr">
+      <c r="AK275" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33611,10 +32784,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK276" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL276" t="inlineStr">
+      <c r="AK276" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33731,10 +32901,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK277" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL277" t="inlineStr">
+      <c r="AK277" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33851,10 +33018,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK278" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL278" t="inlineStr">
+      <c r="AK278" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -33971,10 +33135,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK279" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL279" t="inlineStr">
+      <c r="AK279" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34091,10 +33252,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK280" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL280" t="inlineStr">
+      <c r="AK280" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34211,10 +33369,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK281" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL281" t="inlineStr">
+      <c r="AK281" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34331,10 +33486,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK282" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL282" t="inlineStr">
+      <c r="AK282" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34451,10 +33603,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK283" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL283" t="inlineStr">
+      <c r="AK283" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34571,10 +33720,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK284" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL284" t="inlineStr">
+      <c r="AK284" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34691,10 +33837,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK285" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL285" t="inlineStr">
+      <c r="AK285" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34811,10 +33954,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK286" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL286" t="inlineStr">
+      <c r="AK286" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -34931,10 +34071,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK287" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL287" t="inlineStr">
+      <c r="AK287" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35051,10 +34188,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK288" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL288" t="inlineStr">
+      <c r="AK288" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35171,10 +34305,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK289" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL289" t="inlineStr">
+      <c r="AK289" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35291,10 +34422,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK290" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL290" t="inlineStr">
+      <c r="AK290" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35411,10 +34539,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK291" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL291" t="inlineStr">
+      <c r="AK291" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35531,10 +34656,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK292" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL292" t="inlineStr">
+      <c r="AK292" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35651,10 +34773,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK293" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL293" t="inlineStr">
+      <c r="AK293" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35771,10 +34890,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK294" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL294" t="inlineStr">
+      <c r="AK294" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -35891,10 +35007,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK295" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL295" t="inlineStr">
+      <c r="AK295" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36011,10 +35124,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK296" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL296" t="inlineStr">
+      <c r="AK296" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36131,10 +35241,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK297" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL297" t="inlineStr">
+      <c r="AK297" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36251,10 +35358,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK298" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL298" t="inlineStr">
+      <c r="AK298" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36371,10 +35475,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK299" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL299" t="inlineStr">
+      <c r="AK299" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36491,10 +35592,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK300" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL300" t="inlineStr">
+      <c r="AK300" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36611,10 +35709,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK301" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL301" t="inlineStr">
+      <c r="AK301" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36731,10 +35826,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK302" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL302" t="inlineStr">
+      <c r="AK302" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36851,10 +35943,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK303" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL303" t="inlineStr">
+      <c r="AK303" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -36971,10 +36060,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK304" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL304" t="inlineStr">
+      <c r="AK304" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37091,10 +36177,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK305" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL305" t="inlineStr">
+      <c r="AK305" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37211,10 +36294,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK306" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL306" t="inlineStr">
+      <c r="AK306" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37331,10 +36411,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK307" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL307" t="inlineStr">
+      <c r="AK307" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37451,10 +36528,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK308" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL308" t="inlineStr">
+      <c r="AK308" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37571,10 +36645,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK309" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL309" t="inlineStr">
+      <c r="AK309" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37691,10 +36762,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK310" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL310" t="inlineStr">
+      <c r="AK310" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37811,10 +36879,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK311" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL311" t="inlineStr">
+      <c r="AK311" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -37931,10 +36996,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK312" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL312" t="inlineStr">
+      <c r="AK312" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38051,10 +37113,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK313" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL313" t="inlineStr">
+      <c r="AK313" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38171,10 +37230,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK314" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL314" t="inlineStr">
+      <c r="AK314" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38291,10 +37347,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK315" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL315" t="inlineStr">
+      <c r="AK315" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38411,10 +37464,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK316" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL316" t="inlineStr">
+      <c r="AK316" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38531,10 +37581,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK317" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL317" t="inlineStr">
+      <c r="AK317" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38651,10 +37698,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK318" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL318" t="inlineStr">
+      <c r="AK318" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38771,10 +37815,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK319" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL319" t="inlineStr">
+      <c r="AK319" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -38891,10 +37932,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK320" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL320" t="inlineStr">
+      <c r="AK320" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39011,10 +38049,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK321" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL321" t="inlineStr">
+      <c r="AK321" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39131,10 +38166,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK322" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL322" t="inlineStr">
+      <c r="AK322" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39251,10 +38283,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK323" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL323" t="inlineStr">
+      <c r="AK323" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39371,10 +38400,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK324" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL324" t="inlineStr">
+      <c r="AK324" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39491,10 +38517,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK325" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL325" t="inlineStr">
+      <c r="AK325" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39611,10 +38634,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK326" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL326" t="inlineStr">
+      <c r="AK326" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39731,10 +38751,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK327" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL327" t="inlineStr">
+      <c r="AK327" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39851,10 +38868,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK328" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL328" t="inlineStr">
+      <c r="AK328" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -39971,10 +38985,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK329" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL329" t="inlineStr">
+      <c r="AK329" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40091,10 +39102,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK330" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL330" t="inlineStr">
+      <c r="AK330" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40211,10 +39219,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK331" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL331" t="inlineStr">
+      <c r="AK331" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40331,10 +39336,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK332" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL332" t="inlineStr">
+      <c r="AK332" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40451,10 +39453,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK333" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL333" t="inlineStr">
+      <c r="AK333" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40571,10 +39570,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK334" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL334" t="inlineStr">
+      <c r="AK334" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40691,10 +39687,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK335" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL335" t="inlineStr">
+      <c r="AK335" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40811,10 +39804,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK336" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL336" t="inlineStr">
+      <c r="AK336" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -40931,10 +39921,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK337" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL337" t="inlineStr">
+      <c r="AK337" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41051,10 +40038,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK338" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL338" t="inlineStr">
+      <c r="AK338" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41171,10 +40155,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK339" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL339" t="inlineStr">
+      <c r="AK339" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41291,10 +40272,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK340" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL340" t="inlineStr">
+      <c r="AK340" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41411,10 +40389,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK341" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL341" t="inlineStr">
+      <c r="AK341" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41531,10 +40506,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK342" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL342" t="inlineStr">
+      <c r="AK342" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41651,10 +40623,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK343" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL343" t="inlineStr">
+      <c r="AK343" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41771,10 +40740,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK344" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL344" t="inlineStr">
+      <c r="AK344" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -41891,10 +40857,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK345" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL345" t="inlineStr">
+      <c r="AK345" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -42011,10 +40974,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK346" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL346" t="inlineStr">
+      <c r="AK346" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -42131,10 +41091,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK347" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL347" t="inlineStr">
+      <c r="AK347" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -42251,10 +41208,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK348" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL348" t="inlineStr">
+      <c r="AK348" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -42371,10 +41325,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK349" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL349" t="inlineStr">
+      <c r="AK349" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -42491,10 +41442,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK350" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL350" t="inlineStr">
+      <c r="AK350" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -42611,10 +41559,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK351" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL351" t="inlineStr">
+      <c r="AK351" t="inlineStr">
         <is>
           <t>g</t>
         </is>
@@ -42731,10 +41676,7 @@
           <t>g</t>
         </is>
       </c>
-      <c r="AK352" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL352" t="inlineStr">
+      <c r="AK352" t="inlineStr">
         <is>
           <t>g</t>
         </is>

</xml_diff>